<commit_message>
Manual for the import templates updated for the "specimenCategory" field
</commit_message>
<xml_diff>
--- a/doc/DarwinTemplateSpecimen.xlsx
+++ b/doc/DarwinTemplateSpecimen.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="298">
   <si>
     <t xml:space="preserve">  UnitID</t>
   </si>
@@ -427,9 +427,6 @@
   </si>
   <si>
     <t>Other field information</t>
-  </si>
-  <si>
-    <t>Acqusition</t>
   </si>
   <si>
     <t>Properties</t>
@@ -980,6 +977,18 @@
   </si>
   <si>
     <t>It is also possible to attach a proerty to a collecting station via</t>
+  </si>
+  <si>
+    <t>Acquisition</t>
+  </si>
+  <si>
+    <t>specimenCategory</t>
+  </si>
+  <si>
+    <t>specimens.category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values: "physical"; "observation"; "figurate";"figurate-physical"; "composite-storage-unit" </t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1086,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1134,11 +1143,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1441,10 +1456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I159"/>
+  <dimension ref="A1:I160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,7 +1470,7 @@
     <col min="4" max="4" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="6" width="51.28515625" customWidth="1"/>
-    <col min="7" max="7" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="59.28515625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1466,19 +1481,19 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I1" s="4"/>
     </row>
@@ -1490,16 +1505,16 @@
         <v>131</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I2" s="2"/>
     </row>
@@ -1511,14 +1526,14 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G3"/>
       <c r="H3" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I3" s="2"/>
     </row>
@@ -1530,14 +1545,14 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G4"/>
       <c r="H4" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I4" s="2"/>
     </row>
@@ -1563,16 +1578,16 @@
         <v>78</v>
       </c>
       <c r="E6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G6" t="s">
         <v>161</v>
       </c>
-      <c r="G6" t="s">
-        <v>162</v>
-      </c>
       <c r="H6" s="11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I6" s="2"/>
     </row>
@@ -1586,13 +1601,13 @@
         <v>79</v>
       </c>
       <c r="E7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F7" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" t="s">
         <v>163</v>
-      </c>
-      <c r="G7" t="s">
-        <v>164</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="2"/>
@@ -1607,10 +1622,10 @@
         <v>80</v>
       </c>
       <c r="E8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G8"/>
       <c r="H8" s="11"/>
@@ -1626,10 +1641,10 @@
         <v>81</v>
       </c>
       <c r="E9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G9"/>
       <c r="H9" s="11"/>
@@ -1645,10 +1660,10 @@
         <v>82</v>
       </c>
       <c r="E10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G10"/>
       <c r="H10" s="11"/>
@@ -1664,10 +1679,10 @@
         <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G11"/>
       <c r="H11" s="11"/>
@@ -1683,10 +1698,10 @@
         <v>84</v>
       </c>
       <c r="E12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1699,10 +1714,10 @@
         <v>85</v>
       </c>
       <c r="E13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1715,10 +1730,10 @@
         <v>86</v>
       </c>
       <c r="E14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1731,10 +1746,10 @@
         <v>87</v>
       </c>
       <c r="E15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1747,10 +1762,10 @@
         <v>88</v>
       </c>
       <c r="E16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1763,10 +1778,10 @@
         <v>89</v>
       </c>
       <c r="E17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1779,10 +1794,10 @@
         <v>90</v>
       </c>
       <c r="E18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1801,16 +1816,16 @@
         <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G20" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="H20" s="17" t="s">
         <v>178</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1833,13 +1848,13 @@
         <v>39</v>
       </c>
       <c r="E22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1852,13 +1867,13 @@
         <v>40</v>
       </c>
       <c r="E23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G23">
         <v>1999</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1871,13 +1886,13 @@
         <v>41</v>
       </c>
       <c r="E24" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G24">
         <v>2</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1890,13 +1905,13 @@
         <v>42</v>
       </c>
       <c r="E25" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1909,13 +1924,13 @@
         <v>43</v>
       </c>
       <c r="E26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1928,10 +1943,10 @@
         <v>45</v>
       </c>
       <c r="E27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1944,10 +1959,10 @@
         <v>46</v>
       </c>
       <c r="E28" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F28" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1961,19 +1976,19 @@
         <v>25</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G30">
         <v>1999</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1983,19 +1998,19 @@
         <v>26</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G31">
         <v>3</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2005,19 +2020,19 @@
         <v>27</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F32" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G32">
         <v>4</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2027,19 +2042,19 @@
         <v>28</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2049,19 +2064,19 @@
         <v>29</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2071,19 +2086,19 @@
         <v>30</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F35" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2093,19 +2108,19 @@
         <v>31</v>
       </c>
       <c r="D36" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F36" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G36" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -2128,61 +2143,65 @@
         <v>3</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G38" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="1">
         <v>33</v>
       </c>
-      <c r="D39" t="s">
-        <v>4</v>
+      <c r="D39" s="22" t="s">
+        <v>295</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F39" t="s">
-        <v>200</v>
-      </c>
-      <c r="G39" t="s">
-        <v>148</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="G39" s="31" t="s">
+        <v>297</v>
+      </c>
+      <c r="H39" s="27"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>201</v>
+        <v>154</v>
       </c>
       <c r="F40" t="s">
-        <v>203</v>
+        <v>199</v>
+      </c>
+      <c r="G40" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="F41" t="s">
         <v>202</v>
@@ -2192,347 +2211,346 @@
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E42" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F42" t="s">
         <v>201</v>
-      </c>
-      <c r="F42" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>155</v>
+        <v>200</v>
       </c>
       <c r="F43" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D44" t="s">
-        <v>205</v>
+        <v>8</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>201</v>
+        <v>154</v>
       </c>
       <c r="F44" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>9</v>
+        <v>204</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>155</v>
+        <v>200</v>
       </c>
       <c r="F45" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="1">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D46" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F46" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="1">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F47" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="1">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F48" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="1">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D49" t="s">
-        <v>208</v>
-      </c>
-      <c r="E49" t="s">
-        <v>155</v>
+        <v>27</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>154</v>
       </c>
       <c r="F49" t="s">
-        <v>209</v>
-      </c>
-      <c r="G49" t="s">
-        <v>210</v>
-      </c>
-      <c r="H49" s="13" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D50" t="s">
-        <v>8</v>
+        <v>207</v>
       </c>
       <c r="E50" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F50" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G50" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
+      <c r="C51" s="1">
+        <v>44</v>
+      </c>
+      <c r="D51" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" t="s">
+        <v>154</v>
+      </c>
+      <c r="F51" t="s">
+        <v>211</v>
+      </c>
+      <c r="G51" t="s">
+        <v>212</v>
+      </c>
+      <c r="H51" s="13" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>137</v>
-      </c>
+      <c r="A52" s="3"/>
       <c r="B52" s="3"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
+      <c r="A53" s="3" t="s">
+        <v>294</v>
+      </c>
       <c r="B53" s="3"/>
-      <c r="C53" s="1">
-        <v>45</v>
-      </c>
-      <c r="D53" t="s">
-        <v>16</v>
-      </c>
-      <c r="E53" t="s">
-        <v>155</v>
-      </c>
-      <c r="F53" t="s">
-        <v>219</v>
-      </c>
-      <c r="H53" s="13" t="s">
-        <v>149</v>
-      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D54" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E54" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F54" t="s">
-        <v>226</v>
+        <v>218</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E55" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F55" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E56" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="F56" t="s">
-        <v>228</v>
-      </c>
-      <c r="H56" s="13" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="1">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D57" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E57" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F57" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="H57" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="1">
+        <v>49</v>
+      </c>
+      <c r="D58" t="s">
+        <v>20</v>
+      </c>
+      <c r="E58" t="s">
+        <v>181</v>
+      </c>
+      <c r="F58" t="s">
+        <v>227</v>
+      </c>
+      <c r="H58" s="13" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="1">
         <v>50</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>21</v>
       </c>
-      <c r="E58" t="s">
-        <v>182</v>
-      </c>
-      <c r="F58" t="s">
-        <v>228</v>
-      </c>
-      <c r="H58" s="13" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+      <c r="E59" t="s">
+        <v>181</v>
+      </c>
+      <c r="F59" t="s">
+        <v>227</v>
+      </c>
+      <c r="H59" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B59" s="3"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
-      <c r="C60" s="1">
-        <v>51</v>
-      </c>
-      <c r="D60" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" t="s">
-        <v>230</v>
-      </c>
-      <c r="F60" t="s">
-        <v>231</v>
-      </c>
-      <c r="H60" s="13" t="s">
-        <v>232</v>
-      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D61" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E61" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="F61" t="s">
-        <v>235</v>
+        <v>230</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="1">
-        <v>53</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="G62" s="7"/>
+        <v>52</v>
+      </c>
+      <c r="D62" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" t="s">
+        <v>233</v>
+      </c>
+      <c r="F62" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G63" s="7"/>
     </row>
@@ -2540,378 +2558,377 @@
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="1">
-        <v>55</v>
-      </c>
-      <c r="D64" t="s">
-        <v>22</v>
-      </c>
-      <c r="E64" t="s">
-        <v>238</v>
-      </c>
-      <c r="F64" t="s">
-        <v>239</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="G64" s="7"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="1">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D65" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E65" t="s">
+        <v>237</v>
+      </c>
+      <c r="F65" t="s">
         <v>238</v>
-      </c>
-      <c r="F65" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="1">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D66" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="E66" t="s">
-        <v>182</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
+      </c>
+      <c r="F66" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="1">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D67" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E67" t="s">
-        <v>238</v>
+        <v>181</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="1">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D68" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E68" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="1">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D69" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E69" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>236</v>
-      </c>
-      <c r="G69" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="1">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D70" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E70" t="s">
-        <v>155</v>
-      </c>
-      <c r="F70" s="23" t="s">
-        <v>244</v>
-      </c>
-      <c r="H70" s="13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="G70" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B71" s="3"/>
       <c r="C71" s="1">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D71" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E71" t="s">
-        <v>182</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>237</v>
+        <v>154</v>
+      </c>
+      <c r="F71" s="23" t="s">
+        <v>243</v>
+      </c>
+      <c r="H71" s="13" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B72" s="3"/>
       <c r="C72" s="1">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D72" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E72" t="s">
-        <v>238</v>
+        <v>181</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B73" s="3"/>
       <c r="C73" s="1">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D73" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E73" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B74" s="3"/>
       <c r="C74" s="1">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D74" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E74" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="G74" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B75" s="3"/>
       <c r="C75" s="1">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D75" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E75" t="s">
-        <v>155</v>
-      </c>
-      <c r="F75" s="24" t="s">
-        <v>245</v>
-      </c>
-      <c r="H75" s="13" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="G75" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B76" s="3"/>
       <c r="C76" s="1">
+        <v>66</v>
+      </c>
+      <c r="D76" t="s">
+        <v>59</v>
+      </c>
+      <c r="E76" t="s">
+        <v>154</v>
+      </c>
+      <c r="F76" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="H76" s="13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="3"/>
+      <c r="C77" s="1">
         <v>67</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D77" t="s">
         <v>132</v>
       </c>
-      <c r="E76" t="s">
-        <v>155</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="3" t="s">
+      <c r="E77" t="s">
+        <v>154</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B78" s="3"/>
-      <c r="C78" s="1">
-        <v>68</v>
-      </c>
-      <c r="D78" t="s">
-        <v>60</v>
-      </c>
-      <c r="E78" t="s">
-        <v>201</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="H78" s="13" t="s">
-        <v>220</v>
-      </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B79" s="3"/>
       <c r="C79" s="1">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E79" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="F79" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B80" s="3"/>
       <c r="C80" s="1">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E80" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B81" s="3"/>
       <c r="C81" s="1">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D81" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E81" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>220</v>
+        <v>247</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B82" s="3"/>
       <c r="C82" s="1">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D82" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E82" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>249</v>
+        <v>219</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B83" s="3"/>
       <c r="C83" s="1">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D83" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E83" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F83" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>222</v>
+        <v>248</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B84" s="3"/>
       <c r="C84" s="1">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D84" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E84" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F84" s="7" t="s">
         <v>250</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B85" s="3"/>
       <c r="C85" s="1">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D85" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E85" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F85" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B86" s="3"/>
       <c r="C86" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D86" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E86" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H86" s="13" t="s">
         <v>252</v>
@@ -2920,956 +2937,974 @@
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B87" s="3"/>
       <c r="C87" s="1">
+        <v>76</v>
+      </c>
+      <c r="D87" t="s">
+        <v>68</v>
+      </c>
+      <c r="E87" t="s">
+        <v>200</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="H87" s="13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="3"/>
+      <c r="C88" s="1">
         <v>77</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D88" t="s">
         <v>69</v>
       </c>
-      <c r="E87" t="s">
-        <v>201</v>
-      </c>
-      <c r="F87" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="H87" s="13" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="E88" t="s">
+        <v>200</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="H88" s="13" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B89" s="3"/>
-      <c r="C89" s="1">
-        <v>78</v>
-      </c>
-      <c r="D89" t="s">
-        <v>24</v>
-      </c>
-      <c r="E89" t="s">
-        <v>155</v>
-      </c>
-      <c r="F89" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="H89" s="13" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B90" s="3"/>
       <c r="C90" s="1">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D90" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E90" t="s">
-        <v>158</v>
-      </c>
-      <c r="F90" s="23" t="s">
-        <v>257</v>
+        <v>154</v>
+      </c>
+      <c r="F90" s="7" t="s">
+        <v>253</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B91" s="3"/>
       <c r="C91" s="1">
+        <v>79</v>
+      </c>
+      <c r="D91" t="s">
+        <v>28</v>
+      </c>
+      <c r="E91" t="s">
+        <v>157</v>
+      </c>
+      <c r="F91" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B92" s="3"/>
+      <c r="C92" s="1">
         <v>80</v>
       </c>
-      <c r="D91" t="s">
-        <v>152</v>
-      </c>
-      <c r="E91" t="s">
-        <v>158</v>
-      </c>
-      <c r="F91" s="7" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
+      <c r="D92" t="s">
+        <v>151</v>
+      </c>
+      <c r="E92" t="s">
+        <v>157</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B92" s="3"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="3"/>
       <c r="B93" s="3"/>
-      <c r="C93" s="1">
-        <v>81</v>
-      </c>
-      <c r="D93" t="s">
-        <v>102</v>
-      </c>
-      <c r="E93" t="s">
-        <v>155</v>
-      </c>
-      <c r="F93" t="s">
-        <v>138</v>
-      </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="1">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E94" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F94" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="1">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D95" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E95" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F95" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="1">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D96" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E96" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F96" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B97" s="3"/>
       <c r="C97" s="1">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D97" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E97" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F97" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B98" s="3"/>
       <c r="C98" s="1">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D98" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E98" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F98" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B99" s="3"/>
       <c r="C99" s="1">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D99" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="E99" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F99" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B100" s="3"/>
       <c r="C100" s="1">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D100" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="E100" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F100" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B101" s="3"/>
       <c r="C101" s="1">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D101" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E101" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F101" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B102" s="3"/>
       <c r="C102" s="1">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D102" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E102" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F102" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B103" s="3"/>
       <c r="C103" s="1">
+        <v>90</v>
+      </c>
+      <c r="D103" t="s">
+        <v>110</v>
+      </c>
+      <c r="E103" t="s">
+        <v>154</v>
+      </c>
+      <c r="F103" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B104" s="3"/>
+      <c r="C104" s="1">
         <v>91</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D104" t="s">
         <v>111</v>
       </c>
-      <c r="E103" t="s">
-        <v>155</v>
-      </c>
-      <c r="F103" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="3" t="s">
+      <c r="E104" t="s">
+        <v>154</v>
+      </c>
+      <c r="F104" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B104" s="3"/>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" s="3"/>
       <c r="B105" s="3"/>
-      <c r="C105" s="1">
-        <v>92</v>
-      </c>
-      <c r="D105" t="s">
-        <v>92</v>
-      </c>
-      <c r="E105" t="s">
-        <v>155</v>
-      </c>
-      <c r="F105" t="s">
-        <v>138</v>
-      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="1">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D106" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E106" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F106" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B107" s="3"/>
       <c r="C107" s="1">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D107" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E107" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F107" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B108" s="3"/>
       <c r="C108" s="1">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D108" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E108" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F108" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B109" s="3"/>
       <c r="C109" s="1">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D109" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E109" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F109" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B110" s="3"/>
       <c r="C110" s="1">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D110" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="E110" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F110" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B111" s="3"/>
       <c r="C111" s="1">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D111" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E111" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F111" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B112" s="3"/>
       <c r="C112" s="1">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D112" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="E112" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F112" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B113" s="3"/>
       <c r="C113" s="1">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D113" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E113" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F113" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B114" s="3"/>
       <c r="C114" s="1">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D114" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E114" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F114" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B115" s="3"/>
       <c r="C115" s="1">
+        <v>101</v>
+      </c>
+      <c r="D115" t="s">
+        <v>99</v>
+      </c>
+      <c r="E115" t="s">
+        <v>154</v>
+      </c>
+      <c r="F115" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B116" s="3"/>
+      <c r="C116" s="1">
         <v>102</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D116" t="s">
         <v>100</v>
       </c>
-      <c r="E115" t="s">
-        <v>155</v>
-      </c>
-      <c r="F115" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B116" s="3"/>
+      <c r="E116" t="s">
+        <v>154</v>
+      </c>
+      <c r="F116" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>262</v>
+      </c>
       <c r="B117" s="3"/>
-      <c r="C117" s="1">
-        <v>103</v>
-      </c>
-      <c r="D117" t="s">
-        <v>72</v>
-      </c>
-      <c r="E117" t="s">
-        <v>155</v>
-      </c>
-      <c r="F117" t="s">
-        <v>261</v>
-      </c>
-      <c r="H117" s="13" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B118" s="3"/>
       <c r="C118" s="1">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D118" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E118" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F118" t="s">
+        <v>260</v>
+      </c>
+      <c r="H118" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="H118" s="13" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B119" s="3"/>
       <c r="C119" s="1">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D119" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E119" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F119" t="s">
+        <v>260</v>
+      </c>
+      <c r="H119" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="H119" s="13" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B120" s="3"/>
       <c r="C120" s="1">
+        <v>105</v>
+      </c>
+      <c r="D120" t="s">
+        <v>74</v>
+      </c>
+      <c r="E120" t="s">
+        <v>154</v>
+      </c>
+      <c r="F120" t="s">
+        <v>260</v>
+      </c>
+      <c r="H120" s="13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B121" s="3"/>
+      <c r="C121" s="1">
         <v>106</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D121" t="s">
         <v>75</v>
       </c>
-      <c r="E120" t="s">
-        <v>155</v>
-      </c>
-      <c r="F120" t="s">
+      <c r="E121" t="s">
+        <v>154</v>
+      </c>
+      <c r="F121" t="s">
+        <v>260</v>
+      </c>
+      <c r="H121" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="H120" s="13" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B121" s="3"/>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="B122" s="3"/>
-      <c r="C122" s="1">
-        <v>107</v>
-      </c>
-      <c r="D122" t="s">
-        <v>264</v>
-      </c>
-      <c r="E122" t="s">
-        <v>155</v>
-      </c>
-      <c r="F122" t="s">
-        <v>269</v>
-      </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B123" s="3"/>
       <c r="C123" s="1">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D123" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E123" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F123" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B124" s="3"/>
       <c r="C124" s="1">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D124" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E124" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="F124" t="s">
-        <v>271</v>
-      </c>
-      <c r="H124" s="13" t="s">
-        <v>220</v>
+        <v>269</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B125" s="3"/>
       <c r="C125" s="1">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D125" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E125" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F125" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H125" s="13" t="s">
-        <v>272</v>
+        <v>219</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B126" s="3"/>
       <c r="C126" s="1">
+        <v>110</v>
+      </c>
+      <c r="D126" t="s">
+        <v>266</v>
+      </c>
+      <c r="E126" t="s">
+        <v>181</v>
+      </c>
+      <c r="F126" t="s">
+        <v>270</v>
+      </c>
+      <c r="H126" s="13" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B127" s="3"/>
+      <c r="C127" s="1">
         <v>111</v>
       </c>
-      <c r="D126" t="s">
-        <v>268</v>
-      </c>
-      <c r="E126" t="s">
-        <v>182</v>
-      </c>
-      <c r="F126" t="s">
-        <v>271</v>
-      </c>
-      <c r="H126" s="13" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B127" s="3"/>
+      <c r="D127" t="s">
+        <v>267</v>
+      </c>
+      <c r="E127" t="s">
+        <v>181</v>
+      </c>
+      <c r="F127" t="s">
+        <v>270</v>
+      </c>
+      <c r="H127" s="13" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="B128" s="3"/>
-      <c r="C128" s="1">
-        <v>112</v>
-      </c>
-      <c r="D128" t="s">
-        <v>274</v>
-      </c>
-      <c r="E128" t="s">
-        <v>155</v>
-      </c>
-      <c r="F128" t="s">
-        <v>277</v>
-      </c>
-      <c r="H128" s="13" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B129" s="3"/>
       <c r="C129" s="1">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D129" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E129" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F129" t="s">
+        <v>276</v>
+      </c>
+      <c r="H129" s="13" t="s">
         <v>277</v>
-      </c>
-      <c r="H129" s="13" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B130" s="3"/>
       <c r="C130" s="1">
+        <v>113</v>
+      </c>
+      <c r="D130" t="s">
+        <v>274</v>
+      </c>
+      <c r="E130" t="s">
+        <v>154</v>
+      </c>
+      <c r="F130" t="s">
+        <v>276</v>
+      </c>
+      <c r="H130" s="13" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="3"/>
+      <c r="C131" s="1">
         <v>114</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D131" t="s">
+        <v>275</v>
+      </c>
+      <c r="E131" t="s">
+        <v>154</v>
+      </c>
+      <c r="F131" t="s">
         <v>276</v>
       </c>
-      <c r="E130" t="s">
-        <v>155</v>
-      </c>
-      <c r="F130" t="s">
-        <v>277</v>
-      </c>
-      <c r="H130" s="13" t="s">
+      <c r="H131" s="13" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
+      <c r="B132" s="3"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="3"/>
+      <c r="C133" s="1">
+        <v>115</v>
+      </c>
+      <c r="D133" t="s">
         <v>280</v>
       </c>
-      <c r="B131" s="3"/>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B132" s="3"/>
-      <c r="C132" s="1">
-        <v>115</v>
-      </c>
-      <c r="D132" t="s">
-        <v>281</v>
-      </c>
-      <c r="E132" t="s">
-        <v>155</v>
-      </c>
-      <c r="F132" t="s">
+      <c r="E133" t="s">
+        <v>154</v>
+      </c>
+      <c r="F133" t="s">
+        <v>286</v>
+      </c>
+      <c r="H133" s="13" t="s">
         <v>287</v>
-      </c>
-      <c r="H132" s="13" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C133" s="1">
-        <v>116</v>
-      </c>
-      <c r="D133" t="s">
-        <v>282</v>
-      </c>
-      <c r="E133" t="s">
-        <v>155</v>
-      </c>
-      <c r="F133" t="s">
-        <v>287</v>
-      </c>
-      <c r="H133" s="25" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C134" s="1">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D134" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E134" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F134" t="s">
-        <v>287</v>
-      </c>
-      <c r="H134" s="27" t="s">
-        <v>290</v>
+        <v>286</v>
+      </c>
+      <c r="H134" s="25" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C135" s="1">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D135" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E135" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F135" t="s">
-        <v>287</v>
-      </c>
-      <c r="H135" s="27"/>
+        <v>286</v>
+      </c>
+      <c r="H135" s="28" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C136" s="1">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D136" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E136" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F136" t="s">
         <v>286</v>
       </c>
-      <c r="H136" s="25"/>
+      <c r="H136" s="28"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
-        <v>143</v>
+      <c r="C137" s="1">
+        <v>119</v>
+      </c>
+      <c r="D137" t="s">
+        <v>284</v>
+      </c>
+      <c r="E137" t="s">
+        <v>154</v>
+      </c>
+      <c r="F137" t="s">
+        <v>285</v>
       </c>
       <c r="H137" s="25"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C138" s="1">
+      <c r="A138" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H138" s="25"/>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C139" s="1">
         <v>120</v>
       </c>
-      <c r="D138" t="s">
-        <v>143</v>
-      </c>
-      <c r="E138" t="s">
-        <v>155</v>
-      </c>
-      <c r="F138" t="s">
-        <v>246</v>
-      </c>
-      <c r="H138" s="25"/>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
+      <c r="D139" t="s">
+        <v>142</v>
+      </c>
+      <c r="E139" t="s">
+        <v>154</v>
+      </c>
+      <c r="F139" t="s">
+        <v>245</v>
+      </c>
+      <c r="H139" s="25"/>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D140" s="30"/>
+      <c r="E140" s="30"/>
+      <c r="F140" s="30"/>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D141" s="30" t="s">
+        <v>292</v>
+      </c>
+      <c r="E141" s="30"/>
+      <c r="F141" s="30"/>
+      <c r="G141" s="15"/>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D142" s="25" t="s">
         <v>138</v>
-      </c>
-      <c r="D139" s="29"/>
-      <c r="E139" s="29"/>
-      <c r="F139" s="29"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D140" s="29" t="s">
-        <v>293</v>
-      </c>
-      <c r="E140" s="29"/>
-      <c r="F140" s="29"/>
-      <c r="G140" s="15"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D141" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E141" s="3"/>
-      <c r="F141" s="3"/>
-      <c r="G141" s="15"/>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C142" s="28" t="s">
-        <v>291</v>
-      </c>
-      <c r="D142" s="26" t="s">
-        <v>140</v>
       </c>
       <c r="E142" s="3"/>
       <c r="F142" s="3"/>
       <c r="G142" s="15"/>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C143" s="28"/>
-      <c r="D143" s="25" t="s">
-        <v>141</v>
+      <c r="C143" s="29" t="s">
+        <v>290</v>
+      </c>
+      <c r="D143" s="26" t="s">
+        <v>139</v>
       </c>
       <c r="E143" s="3"/>
       <c r="F143" s="3"/>
       <c r="G143" s="15"/>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D144" s="25"/>
+      <c r="C144" s="29"/>
+      <c r="D144" s="25" t="s">
+        <v>140</v>
+      </c>
       <c r="E144" s="3"/>
       <c r="F144" s="3"/>
       <c r="G144" s="15"/>
     </row>
-    <row r="145" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C145" s="28" t="s">
-        <v>292</v>
-      </c>
-      <c r="D145" s="25" t="s">
-        <v>294</v>
-      </c>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D145" s="25"/>
       <c r="E145" s="3"/>
       <c r="F145" s="3"/>
       <c r="G145" s="15"/>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C146" s="28"/>
-      <c r="D146" s="26" t="s">
-        <v>142</v>
+    <row r="146" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C146" s="29" t="s">
+        <v>291</v>
+      </c>
+      <c r="D146" s="25" t="s">
+        <v>293</v>
       </c>
       <c r="E146" s="3"/>
       <c r="F146" s="3"/>
       <c r="G146" s="15"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B147" s="3"/>
-      <c r="D147" s="16"/>
-      <c r="E147" s="10"/>
-      <c r="F147" s="18"/>
-      <c r="G147" s="10"/>
+      <c r="C147" s="29"/>
+      <c r="D147" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="E147" s="3"/>
+      <c r="F147" s="3"/>
+      <c r="G147" s="15"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A148" s="3"/>
-      <c r="B148" s="20"/>
-      <c r="C148" s="21"/>
-      <c r="D148" s="15"/>
+      <c r="B148" s="3"/>
+      <c r="D148" s="16"/>
+      <c r="E148" s="10"/>
       <c r="F148" s="18"/>
+      <c r="G148" s="10"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A149" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="D149" s="14"/>
+      <c r="A149" s="3"/>
+      <c r="B149" s="20"/>
+      <c r="C149" s="21"/>
+      <c r="D149" s="15"/>
       <c r="F149" s="18"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A150" s="3"/>
-      <c r="B150" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C150"/>
-      <c r="D150" s="18" t="s">
-        <v>177</v>
-      </c>
+      <c r="A150" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="D150" s="14"/>
+      <c r="F150" s="18"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="3"/>
       <c r="B151" s="15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C151"/>
       <c r="D151" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="3"/>
       <c r="B152" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C152"/>
       <c r="D152" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="3"/>
       <c r="B153" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C153"/>
       <c r="D153" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="3"/>
       <c r="B154" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C154"/>
       <c r="D154" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="3"/>
       <c r="B155" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C155"/>
       <c r="D155" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="3"/>
       <c r="B156" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C156"/>
       <c r="D156" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B157" s="16" t="s">
+      <c r="A157" s="3"/>
+      <c r="B157" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C157"/>
+      <c r="D157" s="18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B158" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C157" s="10"/>
-      <c r="D157" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B158" s="15" t="s">
+      <c r="C158" s="10"/>
+      <c r="D158" s="18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B159" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="C158"/>
-      <c r="D158" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B159" s="14" t="s">
-        <v>13</v>
       </c>
       <c r="C159"/>
       <c r="D159" s="18" t="s">
-        <v>233</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B160" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C160"/>
+      <c r="D160" s="18" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="H134:H135"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="D139:F139"/>
+    <mergeCell ref="H135:H136"/>
+    <mergeCell ref="C143:C144"/>
     <mergeCell ref="D140:F140"/>
-    <mergeCell ref="C145:C146"/>
+    <mergeCell ref="D141:F141"/>
+    <mergeCell ref="C146:C147"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>